<commit_message>
add test branches and test code
</commit_message>
<xml_diff>
--- a/test_branch.xlsx
+++ b/test_branch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chueating/Desktop/Projects/AI-Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B581794-0C7A-2F43-A809-5D49C8EB3AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB6DE03-9594-904E-A32D-7C25C409EF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="880" windowWidth="31560" windowHeight="22500" xr2:uid="{88EE7B98-1D16-F34D-B5A6-2979663AE0A5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Correct Answer </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -472,12 +472,233 @@
 This formal proof demonstrates that for any graph, the sum of the degrees of the vertices equals twice the number of edges.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Q7: can you prove that, is the halting problem were decidable, then every r.e. language would be recursive</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the halting problem were decidable, then every r.e.
+language would be recursive. (Thus, the class of r.e. languages and the
+class of recursive languages would be identical.)
+From theorem 12.2, the halting problem is undecidable (since we
+already know that the class of r.e. languages is strictly larger than the
+class of recursive languages.)
+Proof. By de nition, the di erence between r.e. languages and recursive
+languages is that the TM M for an r.e. language L may not halt on an
+input string w when w L while the TM for a recursive language
+always halts on every input string.
+Assume the halting problem is decidable. Consequently, H exists. Then
+we can use H to determine if (Mw) halts. There are two cases to
+consider:
+Case 1. If H decides that (Mw) halts, we can use M to test if w L
+ directly.
+Case 2. If H decides that (Mw) does not halt, then w L.
+H and M together constitute a membership algorithm for L. Hence, L
+is also recursive. We may conclude that all r.e. languages are also
+recursive. This contradicts Theorem 11.5. Hence, the halting problem is
+undecidable.
+In this proof, we construct a membership algorithm for r.e. languages
+based on the the assumed TM H for the halting problem. However, the
+existence of a membership algorithm for the r.e. languages implies all
+r.e. languages are recursive.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certainly! Let's consider the implications of the halting problem being decidable on the class of recursively enumerable (r.e.) languages.
+The halting problem is undecidable, which means that there is no algorithm that can determine, given a Turing machine M and an input w, whether M halts on w or not. Now, let's assume for the sake of contradiction that the halting problem were decidable.
+If the halting problem were decidable, we could construct a decider for the halting problem, let's call it H. This decider H would take as input a description of a Turing machine M and an input w, and it would correctly determine whether M halts on w or not.
+Now, let's consider an arbitrary r.e. language L. By definition, an r.e. language is the language accepted by some Turing machine. Let's call this Turing machine M_L.
+We can construct a new Turing machine M_L', which simulates M_L on input w and then halts if M_L accepts w. Otherwise, it enters an infinite loop. In other words, M_L' halts if and only if M_L accepts w.
+Now, we can use the decider H to determine whether M_L' halts on the empty input ε. If H determines that M_L' halts on ε, then we conclude that M_L accepts ε, and therefore ε is in L. If H determines that M_L' does not halt on ε, then we conclude that M_L does not accept ε, and therefore ε is not in L.
+By repeating this process for all strings in the input alphabet, we can effectively decide whether any given string is in L. This would mean that L is recursive, contradicting the assumption that L is r.e.
+Therefore, if the halting problem were decidable, then every r.e. language would indeed be recursive, which is a contradiction. This demonstrates the profound impact of the undecidability of the halting problem on the class of r.e. languages.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certainly! Let's consider the implications of the halting problem being decidable on the class of recursively enumerable (r.e.) languages, based on the content from Chapter 12. Assuming the halting problem were decidable, we could construct a decider for the halting problem, denoted as H. This decider H would take as input a description of a Turing machine M and an input w, and it would correctly determine whether M halts on w or not. Now, let's consider an arbitrary r.e. language L. By definition, an r.e. language is the language accepted by some Turing machine. Let's call this Turing machine M_L. We can use the decider H to determine whether M_L halts on a given input. If H determines that M_L halts on a specific input, then we can conclude that the input belongs to the language accepted by M_L. If H determines that M_L does not halt on a specific input, then we can conclude that the input does not belong to the language accepted by M_L. By repeating this process for all possible inputs, we can effectively decide membership in L. This would mean that L is recursive, as we have a Turing machine that can decide membership in L. Therefore, if the halting problem were decidable, then every r.e. language would indeed be recursive. This demonstrates the profound impact of the decidability of the halting problem on the class of r.e. languages, as discussed in Chapter 12.</t>
+  </si>
+  <si>
+    <t>Q8: Summarize Introduction to Artificial Intelligence Homework 3.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This homework involves developing Pac-Man agents using various AI strategies: 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Adversarial Search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Implement Minimax and Expectimax algorithms. Modify </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color rgb="FFEB5757"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>multiAgents.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and understand the game logic using supporting files. 2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q-learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Implement Q-learning and value iteration agents. Modify </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color rgb="FFEB5757"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>valueIterationAgents.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color rgb="FFEB5757"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>qlearningAgents.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to calculate optimal policies and Q-values. 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deep Q-Networks (DQN)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Use Deep Reinforcement Learning to improve Pac-Man agents. Modify </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color rgb="FFEB5757"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>DQN.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.199999999999999"/>
+        <color rgb="FFEB5757"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>pacmanDQN_Agents.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and either train your model or use provided pre-trained models. Submit code modifications and a report discussing your implementations and theoretical questions. Follow the submission guidelines to avoid penalties.</t>
+    </r>
+  </si>
+  <si>
+    <t>The homework assignment likely includes specific tasks such as: 1. Implementing the minimax algorithm for decision-making in a competitive environment. 2. Developing an expectimax search algorithm for scenarios with uncertain outcomes. 3. Creating a basic Q-learning agent to learn from its interactions with the environment. 4. Comparing the performance of the Q-learning agent with the provided deep reinforcement learning model (DQN) in a Pac-Man-like environment. Students are expected to gain hands-on experience in implementing these AI algorithms and evaluating their effectiveness in a gaming environment. The assignment likely aims to deepen their understanding of decision-making, learning, and optimization in the context of artificial intelligence.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -532,6 +753,20 @@
       <name val="Segoe UI Symbol"/>
       <family val="2"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.199999999999999"/>
+      <color rgb="FFEB5757"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -899,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D151924-E315-5842-94C1-E2EB2FA6BCBF}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1010,10 +1245,30 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:4">
+    <row r="8" spans="1:4" ht="409.6">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="144">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:4">

</xml_diff>